<commit_message>
Adding new data and odds to the model trainer
Signed-off-by: Supun De Silva <supun1001@gmail.com>
</commit_message>
<xml_diff>
--- a/data_samples/next-week.xlsx
+++ b/data_samples/next-week.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ML101\data_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD848C7-77B6-49A1-9411-58B229804CE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C285594-B948-4D8C-9418-C25197B24FC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23415" yWindow="1365" windowWidth="7095" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -112,13 +112,16 @@
     <t>Home_Team</t>
   </si>
   <si>
-    <t>SCG</t>
+    <t>GMHBA Stadium</t>
   </si>
   <si>
-    <t>Gabba</t>
+    <t>University of Tasmania Stadium</t>
   </si>
   <si>
-    <t>GMHBA Stadium</t>
+    <t>UNSW Canberra Oval</t>
+  </si>
+  <si>
+    <t>Metricon Stadium</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -208,6 +211,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -552,14 +556,14 @@
   <dimension ref="A1:H2278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="4" customWidth="1"/>
     <col min="2" max="3" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="4" customWidth="1"/>
@@ -595,200 +599,182 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14">
+        <v>1.24</v>
+      </c>
+      <c r="H2" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>44311</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1.76</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>44311</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1.66</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>44310</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>32</v>
+      <c r="D5" t="s">
+        <v>22</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5">
-        <v>1.03</v>
+      <c r="G5" s="14">
+        <v>1.1000000000000001</v>
       </c>
-      <c r="H2" s="5">
-        <v>12.5</v>
+      <c r="H5" s="14">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>44304</v>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>44310</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>44304</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5">
-        <v>1.65</v>
-      </c>
-      <c r="H4" s="5">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>44303</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5">
-        <v>1.29</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3.64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>44303</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5">
-        <v>2.1800000000000002</v>
+      <c r="G6" s="14">
+        <v>2.2799999999999998</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.69</v>
+      <c r="H6" s="14">
+        <v>1.75</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>44310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2.34</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>44310</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>44309</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5">
-        <v>1.46</v>
-      </c>
-      <c r="H7" s="5">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>44303</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
+      <c r="D10" s="12" t="s">
+        <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
+      <c r="G10" s="14">
+        <v>3.7</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="H8" s="5">
-        <v>6.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>44302</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5">
-        <v>1.33</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>44301</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5">
-        <v>2.76</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.45</v>
+      <c r="H10" s="14">
+        <v>1.36</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -823,9 +809,9 @@
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
@@ -833,9 +819,9 @@
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
@@ -843,9 +829,9 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
@@ -853,9 +839,9 @@
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="5"/>
@@ -863,9 +849,9 @@
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
@@ -873,9 +859,9 @@
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
@@ -883,9 +869,9 @@
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="5"/>
@@ -893,9 +879,9 @@
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="1"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
@@ -903,9 +889,9 @@
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5"/>

</xml_diff>

<commit_message>
Week 11 data added
Signed-off-by: Supun De Silva <supun1001@gmail.com>
</commit_message>
<xml_diff>
--- a/data_samples/next-week.xlsx
+++ b/data_samples/next-week.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ML101\data_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA0662-C635-4423-BC5A-489415430149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4685F85-E63F-4556-846F-5C92AA833301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31030" yWindow="2900" windowWidth="16650" windowHeight="7280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52790" yWindow="3630" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -43,19 +43,10 @@
     <t>Melbourne</t>
   </si>
   <si>
-    <t>Hawthorn</t>
-  </si>
-  <si>
     <t>Brisbane</t>
   </si>
   <si>
-    <t>North Melbourne</t>
-  </si>
-  <si>
     <t>Essendon</t>
-  </si>
-  <si>
-    <t>Geelong</t>
   </si>
   <si>
     <t>Adelaide</t>
@@ -64,16 +55,7 @@
     <t>Carlton</t>
   </si>
   <si>
-    <t>Port Adelaide</t>
-  </si>
-  <si>
-    <t>Gold Coast</t>
-  </si>
-  <si>
     <t>Richmond</t>
-  </si>
-  <si>
-    <t>GWS Giants</t>
   </si>
   <si>
     <t>Sydney</t>
@@ -112,13 +94,7 @@
     <t>Adelaide Oval</t>
   </si>
   <si>
-    <t>Gabba</t>
-  </si>
-  <si>
     <t>TIO Stadium</t>
-  </si>
-  <si>
-    <t>SCG</t>
   </si>
 </sst>
 </file>
@@ -549,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2213"/>
+  <dimension ref="A1:H2200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,206 +548,152 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
-      <c r="G2" s="5">
-        <v>1.23</v>
-      </c>
-      <c r="H2" s="5">
-        <v>4.2</v>
-      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
-      <c r="G3" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="H3" s="5">
-        <v>2.62</v>
-      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
-        <v>44346</v>
+        <v>44352</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5">
-        <v>1.31</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3.5</v>
-      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
-      <c r="G5" s="5">
-        <v>1.27</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3.78</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>44351</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>31</v>
+      <c r="D7" s="12" t="s">
+        <v>24</v>
       </c>
-      <c r="G6" s="5">
-        <v>1.39</v>
-      </c>
-      <c r="H6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>44345</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.24</v>
-      </c>
-      <c r="H7" s="5">
-        <v>4.0999999999999996</v>
-      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>44345</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="H8" s="5">
-        <v>4.5999999999999996</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>44345</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1.24</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>44344</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="H10" s="5">
-        <v>2.35</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -5567,7 +5489,7 @@
       <c r="A490" s="7"/>
       <c r="B490" s="4"/>
       <c r="C490" s="4"/>
-      <c r="D490" s="1"/>
+      <c r="D490" s="4"/>
       <c r="E490" s="4"/>
       <c r="F490" s="4"/>
       <c r="G490" s="5"/>
@@ -5577,7 +5499,7 @@
       <c r="A491" s="7"/>
       <c r="B491" s="4"/>
       <c r="C491" s="4"/>
-      <c r="D491" s="1"/>
+      <c r="D491" s="4"/>
       <c r="E491" s="4"/>
       <c r="F491" s="4"/>
       <c r="G491" s="5"/>
@@ -5587,7 +5509,7 @@
       <c r="A492" s="7"/>
       <c r="B492" s="4"/>
       <c r="C492" s="4"/>
-      <c r="D492" s="1"/>
+      <c r="D492" s="4"/>
       <c r="E492" s="4"/>
       <c r="F492" s="4"/>
       <c r="G492" s="5"/>
@@ -5597,7 +5519,7 @@
       <c r="A493" s="7"/>
       <c r="B493" s="4"/>
       <c r="C493" s="4"/>
-      <c r="D493" s="1"/>
+      <c r="D493" s="4"/>
       <c r="E493" s="4"/>
       <c r="F493" s="4"/>
       <c r="G493" s="5"/>
@@ -5607,7 +5529,7 @@
       <c r="A494" s="7"/>
       <c r="B494" s="4"/>
       <c r="C494" s="4"/>
-      <c r="D494" s="1"/>
+      <c r="D494" s="4"/>
       <c r="E494" s="4"/>
       <c r="F494" s="4"/>
       <c r="G494" s="5"/>
@@ -5617,7 +5539,7 @@
       <c r="A495" s="7"/>
       <c r="B495" s="4"/>
       <c r="C495" s="4"/>
-      <c r="D495" s="1"/>
+      <c r="D495" s="4"/>
       <c r="E495" s="4"/>
       <c r="F495" s="4"/>
       <c r="G495" s="5"/>
@@ -5627,7 +5549,7 @@
       <c r="A496" s="7"/>
       <c r="B496" s="4"/>
       <c r="C496" s="4"/>
-      <c r="D496" s="1"/>
+      <c r="D496" s="4"/>
       <c r="E496" s="4"/>
       <c r="F496" s="4"/>
       <c r="G496" s="5"/>
@@ -5637,7 +5559,7 @@
       <c r="A497" s="7"/>
       <c r="B497" s="4"/>
       <c r="C497" s="4"/>
-      <c r="D497" s="1"/>
+      <c r="D497" s="4"/>
       <c r="E497" s="4"/>
       <c r="F497" s="4"/>
       <c r="G497" s="5"/>
@@ -5647,7 +5569,7 @@
       <c r="A498" s="7"/>
       <c r="B498" s="4"/>
       <c r="C498" s="4"/>
-      <c r="D498" s="1"/>
+      <c r="D498" s="4"/>
       <c r="E498" s="4"/>
       <c r="F498" s="4"/>
       <c r="G498" s="5"/>
@@ -5657,7 +5579,7 @@
       <c r="A499" s="7"/>
       <c r="B499" s="4"/>
       <c r="C499" s="4"/>
-      <c r="D499" s="1"/>
+      <c r="D499" s="4"/>
       <c r="E499" s="4"/>
       <c r="F499" s="4"/>
       <c r="G499" s="5"/>
@@ -5667,7 +5589,7 @@
       <c r="A500" s="7"/>
       <c r="B500" s="4"/>
       <c r="C500" s="4"/>
-      <c r="D500" s="1"/>
+      <c r="D500" s="4"/>
       <c r="E500" s="4"/>
       <c r="F500" s="4"/>
       <c r="G500" s="5"/>
@@ -5677,7 +5599,7 @@
       <c r="A501" s="7"/>
       <c r="B501" s="4"/>
       <c r="C501" s="4"/>
-      <c r="D501" s="1"/>
+      <c r="D501" s="4"/>
       <c r="E501" s="4"/>
       <c r="F501" s="4"/>
       <c r="G501" s="5"/>
@@ -5687,7 +5609,7 @@
       <c r="A502" s="7"/>
       <c r="B502" s="4"/>
       <c r="C502" s="4"/>
-      <c r="D502" s="1"/>
+      <c r="D502" s="4"/>
       <c r="E502" s="4"/>
       <c r="F502" s="4"/>
       <c r="G502" s="5"/>
@@ -9753,180 +9675,180 @@
       <c r="G908" s="5"/>
       <c r="H908" s="5"/>
     </row>
-    <row r="909" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A909" s="7"/>
-      <c r="B909" s="4"/>
-      <c r="C909" s="4"/>
-      <c r="D909" s="4"/>
-      <c r="E909" s="4"/>
-      <c r="F909" s="4"/>
       <c r="G909" s="5"/>
       <c r="H909" s="5"/>
     </row>
-    <row r="910" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A910" s="7"/>
-      <c r="B910" s="4"/>
-      <c r="C910" s="4"/>
-      <c r="D910" s="4"/>
-      <c r="E910" s="4"/>
-      <c r="F910" s="4"/>
       <c r="G910" s="5"/>
       <c r="H910" s="5"/>
     </row>
-    <row r="911" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A911" s="7"/>
-      <c r="B911" s="4"/>
-      <c r="C911" s="4"/>
-      <c r="D911" s="4"/>
-      <c r="E911" s="4"/>
-      <c r="F911" s="4"/>
       <c r="G911" s="5"/>
       <c r="H911" s="5"/>
     </row>
-    <row r="912" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A912" s="7"/>
-      <c r="B912" s="4"/>
-      <c r="C912" s="4"/>
-      <c r="D912" s="4"/>
-      <c r="E912" s="4"/>
-      <c r="F912" s="4"/>
       <c r="G912" s="5"/>
       <c r="H912" s="5"/>
     </row>
-    <row r="913" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A913" s="7"/>
-      <c r="B913" s="4"/>
-      <c r="C913" s="4"/>
-      <c r="D913" s="4"/>
-      <c r="E913" s="4"/>
-      <c r="F913" s="4"/>
       <c r="G913" s="5"/>
       <c r="H913" s="5"/>
     </row>
-    <row r="914" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A914" s="7"/>
-      <c r="B914" s="4"/>
-      <c r="C914" s="4"/>
-      <c r="D914" s="4"/>
-      <c r="E914" s="4"/>
-      <c r="F914" s="4"/>
       <c r="G914" s="5"/>
       <c r="H914" s="5"/>
     </row>
-    <row r="915" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A915" s="7"/>
-      <c r="B915" s="4"/>
-      <c r="C915" s="4"/>
-      <c r="D915" s="4"/>
-      <c r="E915" s="4"/>
-      <c r="F915" s="4"/>
       <c r="G915" s="5"/>
       <c r="H915" s="5"/>
     </row>
-    <row r="916" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A916" s="7"/>
-      <c r="B916" s="4"/>
-      <c r="C916" s="4"/>
-      <c r="D916" s="4"/>
-      <c r="E916" s="4"/>
-      <c r="F916" s="4"/>
       <c r="G916" s="5"/>
       <c r="H916" s="5"/>
     </row>
-    <row r="917" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A917" s="7"/>
-      <c r="B917" s="4"/>
-      <c r="C917" s="4"/>
-      <c r="D917" s="4"/>
-      <c r="E917" s="4"/>
-      <c r="F917" s="4"/>
       <c r="G917" s="5"/>
       <c r="H917" s="5"/>
     </row>
     <row r="918" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A918" s="7"/>
-      <c r="B918" s="4"/>
-      <c r="C918" s="4"/>
-      <c r="D918" s="4"/>
-      <c r="E918" s="4"/>
-      <c r="F918" s="4"/>
-      <c r="G918" s="5"/>
-      <c r="H918" s="5"/>
+      <c r="B918" s="6"/>
+      <c r="C918" s="6"/>
+      <c r="D918" s="6"/>
+      <c r="E918" s="6"/>
+      <c r="F918" s="6"/>
+      <c r="G918" s="8"/>
+      <c r="H918" s="8"/>
     </row>
     <row r="919" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A919" s="7"/>
-      <c r="B919" s="4"/>
-      <c r="C919" s="4"/>
-      <c r="D919" s="4"/>
-      <c r="E919" s="4"/>
-      <c r="F919" s="4"/>
-      <c r="G919" s="5"/>
-      <c r="H919" s="5"/>
+      <c r="B919" s="6"/>
+      <c r="C919" s="6"/>
+      <c r="D919" s="6"/>
+      <c r="E919" s="6"/>
+      <c r="F919" s="6"/>
+      <c r="G919" s="8"/>
+      <c r="H919" s="8"/>
     </row>
     <row r="920" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A920" s="7"/>
-      <c r="B920" s="4"/>
-      <c r="C920" s="4"/>
-      <c r="D920" s="4"/>
-      <c r="E920" s="4"/>
-      <c r="F920" s="4"/>
-      <c r="G920" s="5"/>
-      <c r="H920" s="5"/>
+      <c r="B920" s="6"/>
+      <c r="C920" s="6"/>
+      <c r="D920" s="6"/>
+      <c r="E920" s="6"/>
+      <c r="F920" s="6"/>
+      <c r="G920" s="8"/>
+      <c r="H920" s="8"/>
     </row>
     <row r="921" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A921" s="7"/>
-      <c r="B921" s="4"/>
-      <c r="C921" s="4"/>
-      <c r="D921" s="4"/>
-      <c r="E921" s="4"/>
-      <c r="F921" s="4"/>
-      <c r="G921" s="5"/>
-      <c r="H921" s="5"/>
-    </row>
-    <row r="922" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B921" s="6"/>
+      <c r="C921" s="6"/>
+      <c r="D921" s="6"/>
+      <c r="E921" s="6"/>
+      <c r="F921" s="6"/>
+      <c r="G921" s="8"/>
+      <c r="H921" s="8"/>
+    </row>
+    <row r="922" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A922" s="7"/>
-      <c r="G922" s="5"/>
-      <c r="H922" s="5"/>
-    </row>
-    <row r="923" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B922" s="6"/>
+      <c r="C922" s="6"/>
+      <c r="D922" s="6"/>
+      <c r="E922" s="6"/>
+      <c r="F922" s="6"/>
+      <c r="G922" s="8"/>
+      <c r="H922" s="8"/>
+    </row>
+    <row r="923" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A923" s="7"/>
-      <c r="G923" s="5"/>
-      <c r="H923" s="5"/>
-    </row>
-    <row r="924" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B923" s="6"/>
+      <c r="C923" s="6"/>
+      <c r="D923" s="6"/>
+      <c r="E923" s="6"/>
+      <c r="F923" s="6"/>
+      <c r="G923" s="8"/>
+      <c r="H923" s="8"/>
+    </row>
+    <row r="924" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A924" s="7"/>
-      <c r="G924" s="5"/>
-      <c r="H924" s="5"/>
-    </row>
-    <row r="925" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B924" s="6"/>
+      <c r="C924" s="6"/>
+      <c r="D924" s="6"/>
+      <c r="E924" s="6"/>
+      <c r="F924" s="6"/>
+      <c r="G924" s="8"/>
+      <c r="H924" s="8"/>
+    </row>
+    <row r="925" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A925" s="7"/>
-      <c r="G925" s="5"/>
-      <c r="H925" s="5"/>
-    </row>
-    <row r="926" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B925" s="6"/>
+      <c r="C925" s="6"/>
+      <c r="D925" s="6"/>
+      <c r="E925" s="6"/>
+      <c r="F925" s="6"/>
+      <c r="G925" s="8"/>
+      <c r="H925" s="8"/>
+    </row>
+    <row r="926" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A926" s="7"/>
-      <c r="G926" s="5"/>
-      <c r="H926" s="5"/>
-    </row>
-    <row r="927" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B926" s="6"/>
+      <c r="C926" s="6"/>
+      <c r="D926" s="6"/>
+      <c r="E926" s="6"/>
+      <c r="F926" s="6"/>
+      <c r="G926" s="8"/>
+      <c r="H926" s="8"/>
+    </row>
+    <row r="927" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A927" s="7"/>
-      <c r="G927" s="5"/>
-      <c r="H927" s="5"/>
-    </row>
-    <row r="928" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B927" s="6"/>
+      <c r="C927" s="6"/>
+      <c r="D927" s="6"/>
+      <c r="E927" s="6"/>
+      <c r="F927" s="6"/>
+      <c r="G927" s="8"/>
+      <c r="H927" s="8"/>
+    </row>
+    <row r="928" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A928" s="7"/>
-      <c r="G928" s="5"/>
-      <c r="H928" s="5"/>
-    </row>
-    <row r="929" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B928" s="6"/>
+      <c r="C928" s="6"/>
+      <c r="D928" s="6"/>
+      <c r="E928" s="6"/>
+      <c r="F928" s="6"/>
+      <c r="G928" s="8"/>
+      <c r="H928" s="8"/>
+    </row>
+    <row r="929" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A929" s="7"/>
-      <c r="G929" s="5"/>
-      <c r="H929" s="5"/>
-    </row>
-    <row r="930" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B929" s="6"/>
+      <c r="C929" s="6"/>
+      <c r="D929" s="6"/>
+      <c r="E929" s="6"/>
+      <c r="F929" s="6"/>
+      <c r="G929" s="8"/>
+      <c r="H929" s="8"/>
+    </row>
+    <row r="930" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A930" s="7"/>
-      <c r="G930" s="5"/>
-      <c r="H930" s="5"/>
+      <c r="B930" s="6"/>
+      <c r="C930" s="6"/>
+      <c r="D930" s="6"/>
+      <c r="E930" s="6"/>
+      <c r="F930" s="6"/>
+      <c r="G930" s="8"/>
+      <c r="H930" s="8"/>
     </row>
     <row r="931" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A931" s="7"/>
@@ -15188,7 +15110,7 @@
       <c r="G1456" s="8"/>
       <c r="H1456" s="8"/>
     </row>
-    <row r="1457" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1457" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1457" s="7"/>
       <c r="B1457" s="6"/>
       <c r="C1457" s="6"/>
@@ -15198,7 +15120,7 @@
       <c r="G1457" s="8"/>
       <c r="H1457" s="8"/>
     </row>
-    <row r="1458" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1458" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1458" s="7"/>
       <c r="B1458" s="6"/>
       <c r="C1458" s="6"/>
@@ -15208,7 +15130,7 @@
       <c r="G1458" s="8"/>
       <c r="H1458" s="8"/>
     </row>
-    <row r="1459" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1459" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1459" s="7"/>
       <c r="B1459" s="6"/>
       <c r="C1459" s="6"/>
@@ -15218,7 +15140,7 @@
       <c r="G1459" s="8"/>
       <c r="H1459" s="8"/>
     </row>
-    <row r="1460" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1460" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1460" s="7"/>
       <c r="B1460" s="6"/>
       <c r="C1460" s="6"/>
@@ -15228,7 +15150,7 @@
       <c r="G1460" s="8"/>
       <c r="H1460" s="8"/>
     </row>
-    <row r="1461" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1461" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1461" s="7"/>
       <c r="B1461" s="6"/>
       <c r="C1461" s="6"/>
@@ -15238,7 +15160,7 @@
       <c r="G1461" s="8"/>
       <c r="H1461" s="8"/>
     </row>
-    <row r="1462" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1462" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1462" s="7"/>
       <c r="B1462" s="6"/>
       <c r="C1462" s="6"/>
@@ -15248,7 +15170,7 @@
       <c r="G1462" s="8"/>
       <c r="H1462" s="8"/>
     </row>
-    <row r="1463" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1463" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1463" s="7"/>
       <c r="B1463" s="6"/>
       <c r="C1463" s="6"/>
@@ -15258,7 +15180,7 @@
       <c r="G1463" s="8"/>
       <c r="H1463" s="8"/>
     </row>
-    <row r="1464" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1464" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1464" s="7"/>
       <c r="B1464" s="6"/>
       <c r="C1464" s="6"/>
@@ -15268,7 +15190,7 @@
       <c r="G1464" s="8"/>
       <c r="H1464" s="8"/>
     </row>
-    <row r="1465" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1465" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1465" s="7"/>
       <c r="B1465" s="6"/>
       <c r="C1465" s="6"/>
@@ -15318,7 +15240,7 @@
       <c r="G1469" s="8"/>
       <c r="H1469" s="8"/>
     </row>
-    <row r="1470" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1470" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1470" s="7"/>
       <c r="B1470" s="6"/>
       <c r="C1470" s="6"/>
@@ -15328,7 +15250,7 @@
       <c r="G1470" s="8"/>
       <c r="H1470" s="8"/>
     </row>
-    <row r="1471" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1471" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1471" s="7"/>
       <c r="B1471" s="6"/>
       <c r="C1471" s="6"/>
@@ -15338,7 +15260,7 @@
       <c r="G1471" s="8"/>
       <c r="H1471" s="8"/>
     </row>
-    <row r="1472" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1472" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1472" s="7"/>
       <c r="B1472" s="6"/>
       <c r="C1472" s="6"/>
@@ -15348,7 +15270,7 @@
       <c r="G1472" s="8"/>
       <c r="H1472" s="8"/>
     </row>
-    <row r="1473" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1473" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1473" s="7"/>
       <c r="B1473" s="6"/>
       <c r="C1473" s="6"/>
@@ -15358,7 +15280,7 @@
       <c r="G1473" s="8"/>
       <c r="H1473" s="8"/>
     </row>
-    <row r="1474" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1474" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1474" s="7"/>
       <c r="B1474" s="6"/>
       <c r="C1474" s="6"/>
@@ -15368,7 +15290,7 @@
       <c r="G1474" s="8"/>
       <c r="H1474" s="8"/>
     </row>
-    <row r="1475" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1475" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1475" s="7"/>
       <c r="B1475" s="6"/>
       <c r="C1475" s="6"/>
@@ -15378,7 +15300,7 @@
       <c r="G1475" s="8"/>
       <c r="H1475" s="8"/>
     </row>
-    <row r="1476" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1476" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1476" s="7"/>
       <c r="B1476" s="6"/>
       <c r="C1476" s="6"/>
@@ -15388,7 +15310,7 @@
       <c r="G1476" s="8"/>
       <c r="H1476" s="8"/>
     </row>
-    <row r="1477" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1477" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1477" s="7"/>
       <c r="B1477" s="6"/>
       <c r="C1477" s="6"/>
@@ -15398,7 +15320,7 @@
       <c r="G1477" s="8"/>
       <c r="H1477" s="8"/>
     </row>
-    <row r="1478" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1478" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1478" s="7"/>
       <c r="B1478" s="6"/>
       <c r="C1478" s="6"/>
@@ -15819,134 +15741,134 @@
       <c r="H1519" s="8"/>
     </row>
     <row r="1520" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1520" s="7"/>
-      <c r="B1520" s="6"/>
-      <c r="C1520" s="6"/>
-      <c r="D1520" s="6"/>
-      <c r="E1520" s="6"/>
-      <c r="F1520" s="6"/>
-      <c r="G1520" s="8"/>
-      <c r="H1520" s="8"/>
+      <c r="A1520" s="3"/>
+      <c r="B1520" s="4"/>
+      <c r="C1520" s="4"/>
+      <c r="D1520" s="4"/>
+      <c r="E1520" s="4"/>
+      <c r="F1520" s="4"/>
+      <c r="G1520" s="5"/>
+      <c r="H1520" s="5"/>
     </row>
     <row r="1521" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1521" s="7"/>
-      <c r="B1521" s="6"/>
-      <c r="C1521" s="6"/>
-      <c r="D1521" s="6"/>
-      <c r="E1521" s="6"/>
-      <c r="F1521" s="6"/>
-      <c r="G1521" s="8"/>
-      <c r="H1521" s="8"/>
+      <c r="A1521" s="3"/>
+      <c r="B1521" s="4"/>
+      <c r="C1521" s="4"/>
+      <c r="D1521" s="4"/>
+      <c r="E1521" s="4"/>
+      <c r="F1521" s="4"/>
+      <c r="G1521" s="5"/>
+      <c r="H1521" s="5"/>
     </row>
     <row r="1522" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1522" s="7"/>
-      <c r="B1522" s="6"/>
-      <c r="C1522" s="6"/>
-      <c r="D1522" s="6"/>
-      <c r="E1522" s="6"/>
-      <c r="F1522" s="6"/>
-      <c r="G1522" s="8"/>
-      <c r="H1522" s="8"/>
+      <c r="A1522" s="3"/>
+      <c r="B1522" s="4"/>
+      <c r="C1522" s="4"/>
+      <c r="D1522" s="4"/>
+      <c r="E1522" s="4"/>
+      <c r="F1522" s="4"/>
+      <c r="G1522" s="5"/>
+      <c r="H1522" s="5"/>
     </row>
     <row r="1523" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1523" s="7"/>
-      <c r="B1523" s="6"/>
-      <c r="C1523" s="6"/>
-      <c r="D1523" s="6"/>
-      <c r="E1523" s="6"/>
-      <c r="F1523" s="6"/>
-      <c r="G1523" s="8"/>
-      <c r="H1523" s="8"/>
+      <c r="A1523" s="3"/>
+      <c r="B1523" s="4"/>
+      <c r="C1523" s="4"/>
+      <c r="D1523" s="4"/>
+      <c r="E1523" s="4"/>
+      <c r="F1523" s="4"/>
+      <c r="G1523" s="5"/>
+      <c r="H1523" s="5"/>
     </row>
     <row r="1524" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1524" s="7"/>
-      <c r="B1524" s="6"/>
-      <c r="C1524" s="6"/>
-      <c r="D1524" s="6"/>
-      <c r="E1524" s="6"/>
-      <c r="F1524" s="6"/>
-      <c r="G1524" s="8"/>
-      <c r="H1524" s="8"/>
+      <c r="A1524" s="3"/>
+      <c r="B1524" s="4"/>
+      <c r="C1524" s="4"/>
+      <c r="D1524" s="4"/>
+      <c r="E1524" s="4"/>
+      <c r="F1524" s="4"/>
+      <c r="G1524" s="5"/>
+      <c r="H1524" s="5"/>
     </row>
     <row r="1525" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1525" s="7"/>
-      <c r="B1525" s="6"/>
-      <c r="C1525" s="6"/>
-      <c r="D1525" s="6"/>
-      <c r="E1525" s="6"/>
-      <c r="F1525" s="6"/>
-      <c r="G1525" s="8"/>
-      <c r="H1525" s="8"/>
+      <c r="A1525" s="3"/>
+      <c r="B1525" s="4"/>
+      <c r="C1525" s="4"/>
+      <c r="D1525" s="4"/>
+      <c r="E1525" s="4"/>
+      <c r="F1525" s="4"/>
+      <c r="G1525" s="5"/>
+      <c r="H1525" s="5"/>
     </row>
     <row r="1526" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1526" s="7"/>
-      <c r="B1526" s="6"/>
-      <c r="C1526" s="6"/>
-      <c r="D1526" s="6"/>
-      <c r="E1526" s="6"/>
-      <c r="F1526" s="6"/>
-      <c r="G1526" s="8"/>
-      <c r="H1526" s="8"/>
+      <c r="A1526" s="3"/>
+      <c r="B1526" s="4"/>
+      <c r="C1526" s="4"/>
+      <c r="D1526" s="4"/>
+      <c r="E1526" s="4"/>
+      <c r="F1526" s="4"/>
+      <c r="G1526" s="5"/>
+      <c r="H1526" s="5"/>
     </row>
     <row r="1527" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1527" s="7"/>
-      <c r="B1527" s="6"/>
-      <c r="C1527" s="6"/>
-      <c r="D1527" s="6"/>
-      <c r="E1527" s="6"/>
-      <c r="F1527" s="6"/>
-      <c r="G1527" s="8"/>
-      <c r="H1527" s="8"/>
+      <c r="A1527" s="3"/>
+      <c r="B1527" s="4"/>
+      <c r="C1527" s="4"/>
+      <c r="D1527" s="4"/>
+      <c r="E1527" s="4"/>
+      <c r="F1527" s="4"/>
+      <c r="G1527" s="5"/>
+      <c r="H1527" s="5"/>
     </row>
     <row r="1528" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1528" s="7"/>
-      <c r="B1528" s="6"/>
-      <c r="C1528" s="6"/>
-      <c r="D1528" s="6"/>
-      <c r="E1528" s="6"/>
-      <c r="F1528" s="6"/>
-      <c r="G1528" s="8"/>
-      <c r="H1528" s="8"/>
+      <c r="A1528" s="3"/>
+      <c r="B1528" s="4"/>
+      <c r="C1528" s="4"/>
+      <c r="D1528" s="4"/>
+      <c r="E1528" s="4"/>
+      <c r="F1528" s="4"/>
+      <c r="G1528" s="5"/>
+      <c r="H1528" s="5"/>
     </row>
     <row r="1529" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1529" s="7"/>
-      <c r="B1529" s="6"/>
-      <c r="C1529" s="6"/>
-      <c r="D1529" s="6"/>
-      <c r="E1529" s="6"/>
-      <c r="F1529" s="6"/>
-      <c r="G1529" s="8"/>
-      <c r="H1529" s="8"/>
+      <c r="A1529" s="3"/>
+      <c r="B1529" s="4"/>
+      <c r="C1529" s="4"/>
+      <c r="D1529" s="4"/>
+      <c r="E1529" s="4"/>
+      <c r="F1529" s="4"/>
+      <c r="G1529" s="5"/>
+      <c r="H1529" s="5"/>
     </row>
     <row r="1530" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1530" s="7"/>
-      <c r="B1530" s="6"/>
-      <c r="C1530" s="6"/>
-      <c r="D1530" s="6"/>
-      <c r="E1530" s="6"/>
-      <c r="F1530" s="6"/>
-      <c r="G1530" s="8"/>
-      <c r="H1530" s="8"/>
+      <c r="A1530" s="3"/>
+      <c r="B1530" s="4"/>
+      <c r="C1530" s="4"/>
+      <c r="D1530" s="4"/>
+      <c r="E1530" s="4"/>
+      <c r="F1530" s="4"/>
+      <c r="G1530" s="5"/>
+      <c r="H1530" s="5"/>
     </row>
     <row r="1531" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1531" s="7"/>
-      <c r="B1531" s="6"/>
-      <c r="C1531" s="6"/>
-      <c r="D1531" s="6"/>
-      <c r="E1531" s="6"/>
-      <c r="F1531" s="6"/>
-      <c r="G1531" s="8"/>
-      <c r="H1531" s="8"/>
+      <c r="A1531" s="3"/>
+      <c r="B1531" s="4"/>
+      <c r="C1531" s="4"/>
+      <c r="D1531" s="4"/>
+      <c r="E1531" s="4"/>
+      <c r="F1531" s="4"/>
+      <c r="G1531" s="5"/>
+      <c r="H1531" s="5"/>
     </row>
     <row r="1532" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1532" s="7"/>
-      <c r="B1532" s="6"/>
-      <c r="C1532" s="6"/>
-      <c r="D1532" s="6"/>
-      <c r="E1532" s="6"/>
-      <c r="F1532" s="6"/>
-      <c r="G1532" s="8"/>
-      <c r="H1532" s="8"/>
+      <c r="A1532" s="3"/>
+      <c r="B1532" s="4"/>
+      <c r="C1532" s="4"/>
+      <c r="D1532" s="4"/>
+      <c r="E1532" s="4"/>
+      <c r="F1532" s="4"/>
+      <c r="G1532" s="5"/>
+      <c r="H1532" s="5"/>
     </row>
     <row r="1533" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1533" s="3"/>
@@ -17833,7 +17755,7 @@
       <c r="B1721" s="4"/>
       <c r="C1721" s="4"/>
       <c r="D1721" s="4"/>
-      <c r="E1721" s="4"/>
+      <c r="E1721" s="6"/>
       <c r="F1721" s="4"/>
       <c r="G1721" s="5"/>
       <c r="H1721" s="5"/>
@@ -17888,133 +17810,68 @@
       <c r="G1726" s="5"/>
       <c r="H1726" s="5"/>
     </row>
-    <row r="1727" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1727" s="3"/>
-      <c r="B1727" s="4"/>
-      <c r="C1727" s="4"/>
-      <c r="D1727" s="4"/>
-      <c r="E1727" s="4"/>
-      <c r="F1727" s="4"/>
       <c r="G1727" s="5"/>
       <c r="H1727" s="5"/>
     </row>
-    <row r="1728" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1728" s="3"/>
-      <c r="B1728" s="4"/>
-      <c r="C1728" s="4"/>
-      <c r="D1728" s="4"/>
-      <c r="E1728" s="4"/>
-      <c r="F1728" s="4"/>
       <c r="G1728" s="5"/>
       <c r="H1728" s="5"/>
     </row>
-    <row r="1729" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1729" s="3"/>
-      <c r="B1729" s="4"/>
-      <c r="C1729" s="4"/>
-      <c r="D1729" s="4"/>
-      <c r="E1729" s="4"/>
-      <c r="F1729" s="4"/>
       <c r="G1729" s="5"/>
       <c r="H1729" s="5"/>
     </row>
-    <row r="1730" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1730" s="3"/>
-      <c r="B1730" s="4"/>
-      <c r="C1730" s="4"/>
-      <c r="D1730" s="4"/>
-      <c r="E1730" s="4"/>
-      <c r="F1730" s="4"/>
       <c r="G1730" s="5"/>
       <c r="H1730" s="5"/>
     </row>
-    <row r="1731" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1731" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1731" s="3"/>
-      <c r="B1731" s="4"/>
-      <c r="C1731" s="4"/>
-      <c r="D1731" s="4"/>
-      <c r="E1731" s="4"/>
-      <c r="F1731" s="4"/>
       <c r="G1731" s="5"/>
       <c r="H1731" s="5"/>
     </row>
-    <row r="1732" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1732" s="3"/>
-      <c r="B1732" s="4"/>
-      <c r="C1732" s="4"/>
-      <c r="D1732" s="4"/>
-      <c r="E1732" s="4"/>
-      <c r="F1732" s="4"/>
       <c r="G1732" s="5"/>
       <c r="H1732" s="5"/>
     </row>
-    <row r="1733" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1733" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1733" s="3"/>
-      <c r="B1733" s="4"/>
-      <c r="C1733" s="4"/>
-      <c r="D1733" s="4"/>
-      <c r="E1733" s="4"/>
-      <c r="F1733" s="4"/>
       <c r="G1733" s="5"/>
       <c r="H1733" s="5"/>
     </row>
-    <row r="1734" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1734" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1734" s="3"/>
-      <c r="B1734" s="4"/>
-      <c r="C1734" s="4"/>
-      <c r="D1734" s="4"/>
-      <c r="E1734" s="6"/>
-      <c r="F1734" s="4"/>
       <c r="G1734" s="5"/>
       <c r="H1734" s="5"/>
     </row>
-    <row r="1735" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1735" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1735" s="3"/>
-      <c r="B1735" s="4"/>
-      <c r="C1735" s="4"/>
-      <c r="D1735" s="4"/>
-      <c r="E1735" s="4"/>
-      <c r="F1735" s="4"/>
       <c r="G1735" s="5"/>
       <c r="H1735" s="5"/>
     </row>
-    <row r="1736" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1736" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1736" s="3"/>
-      <c r="B1736" s="4"/>
-      <c r="C1736" s="4"/>
-      <c r="D1736" s="4"/>
-      <c r="E1736" s="4"/>
-      <c r="F1736" s="4"/>
       <c r="G1736" s="5"/>
       <c r="H1736" s="5"/>
     </row>
-    <row r="1737" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1737" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1737" s="3"/>
-      <c r="B1737" s="4"/>
-      <c r="C1737" s="4"/>
-      <c r="D1737" s="4"/>
-      <c r="E1737" s="4"/>
-      <c r="F1737" s="4"/>
       <c r="G1737" s="5"/>
       <c r="H1737" s="5"/>
     </row>
-    <row r="1738" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1738" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1738" s="3"/>
-      <c r="B1738" s="4"/>
-      <c r="C1738" s="4"/>
-      <c r="D1738" s="4"/>
-      <c r="E1738" s="4"/>
-      <c r="F1738" s="4"/>
       <c r="G1738" s="5"/>
       <c r="H1738" s="5"/>
     </row>
-    <row r="1739" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1739" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1739" s="3"/>
-      <c r="B1739" s="4"/>
-      <c r="C1739" s="4"/>
-      <c r="D1739" s="4"/>
-      <c r="E1739" s="4"/>
-      <c r="F1739" s="4"/>
       <c r="G1739" s="5"/>
       <c r="H1739" s="5"/>
     </row>
@@ -20323,74 +20180,9 @@
       <c r="G2200" s="5"/>
       <c r="H2200" s="5"/>
     </row>
-    <row r="2201" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2201" s="3"/>
-      <c r="G2201" s="5"/>
-      <c r="H2201" s="5"/>
-    </row>
-    <row r="2202" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2202" s="3"/>
-      <c r="G2202" s="5"/>
-      <c r="H2202" s="5"/>
-    </row>
-    <row r="2203" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2203" s="3"/>
-      <c r="G2203" s="5"/>
-      <c r="H2203" s="5"/>
-    </row>
-    <row r="2204" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2204" s="3"/>
-      <c r="G2204" s="5"/>
-      <c r="H2204" s="5"/>
-    </row>
-    <row r="2205" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2205" s="3"/>
-      <c r="G2205" s="5"/>
-      <c r="H2205" s="5"/>
-    </row>
-    <row r="2206" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2206" s="3"/>
-      <c r="G2206" s="5"/>
-      <c r="H2206" s="5"/>
-    </row>
-    <row r="2207" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2207" s="3"/>
-      <c r="G2207" s="5"/>
-      <c r="H2207" s="5"/>
-    </row>
-    <row r="2208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2208" s="3"/>
-      <c r="G2208" s="5"/>
-      <c r="H2208" s="5"/>
-    </row>
-    <row r="2209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2209" s="3"/>
-      <c r="G2209" s="5"/>
-      <c r="H2209" s="5"/>
-    </row>
-    <row r="2210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2210" s="3"/>
-      <c r="G2210" s="5"/>
-      <c r="H2210" s="5"/>
-    </row>
-    <row r="2211" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2211" s="3"/>
-      <c r="G2211" s="5"/>
-      <c r="H2211" s="5"/>
-    </row>
-    <row r="2212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2212" s="3"/>
-      <c r="G2212" s="5"/>
-      <c r="H2212" s="5"/>
-    </row>
-    <row r="2213" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2213" s="3"/>
-      <c r="G2213" s="5"/>
-      <c r="H2213" s="5"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H395">
-    <sortCondition descending="1" ref="A1:A395"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H382">
+    <sortCondition descending="1" ref="A1:A382"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Run History, Multi Threaded
Signed-off-by: Supun De Silva <supun1001@gmail.com>
</commit_message>
<xml_diff>
--- a/data_samples/next-week.xlsx
+++ b/data_samples/next-week.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ML101\data_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1743F7EE-7FBD-44F1-B84F-071EB8F498E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997FE503-B0E0-43C1-BE85-871F64170A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12980" yWindow="8340" windowWidth="19440" windowHeight="8900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -109,16 +109,13 @@
     <t>Adelaide</t>
   </si>
   <si>
-    <t>GMHBA Stadium</t>
-  </si>
-  <si>
-    <t>University of Tasmania Stadium</t>
-  </si>
-  <si>
     <t>Mars Stadium</t>
   </si>
   <si>
     <t>Optus Stadium</t>
+  </si>
+  <si>
+    <t>Metricon Stadium</t>
   </si>
 </sst>
 </file>
@@ -549,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2156"/>
+  <dimension ref="A1:H2132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,182 +592,191 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
-        <v>44389</v>
+        <v>44395</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="D2" s="12" t="s">
+        <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="5">
-        <v>1.18</v>
+        <v>2.15</v>
       </c>
       <c r="H2" s="5">
-        <v>4.95</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="5">
-        <v>1.57</v>
+        <v>1.95</v>
       </c>
       <c r="H3" s="5">
-        <v>2.42</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>1.3</v>
+        <v>3.1</v>
       </c>
       <c r="H4" s="5">
-        <v>3.56</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
-        <v>44388</v>
+        <v>44394</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
+        <v>1.95</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>44394</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>44394</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>44394</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>31</v>
+      <c r="D8" s="12" t="s">
+        <v>29</v>
       </c>
-      <c r="G5" s="5">
-        <v>1.37</v>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5">
+        <v>2.5499999999999998</v>
       </c>
-      <c r="H5" s="5">
-        <v>3.3</v>
+      <c r="H8" s="5">
+        <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>44387</v>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>44393</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
+        <v>2.71</v>
       </c>
-      <c r="G6" s="5">
-        <v>1.22</v>
+      <c r="H9" s="5">
+        <v>1.47</v>
       </c>
-      <c r="H6" s="5">
-        <v>4.3</v>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>44392</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>44387</v>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="5">
-        <v>3.72</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>44387</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="5">
-        <v>2.19</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>44386</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.28</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3.73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>44385</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="5">
-        <v>1.69</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H10" s="5">
-        <v>2.1800000000000002</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4887,7 +4893,7 @@
       <c r="A422" s="7"/>
       <c r="B422" s="4"/>
       <c r="C422" s="4"/>
-      <c r="D422" s="1"/>
+      <c r="D422" s="4"/>
       <c r="E422" s="4"/>
       <c r="F422" s="4"/>
       <c r="G422" s="5"/>
@@ -4897,7 +4903,7 @@
       <c r="A423" s="7"/>
       <c r="B423" s="4"/>
       <c r="C423" s="4"/>
-      <c r="D423" s="1"/>
+      <c r="D423" s="4"/>
       <c r="E423" s="4"/>
       <c r="F423" s="4"/>
       <c r="G423" s="5"/>
@@ -4907,7 +4913,7 @@
       <c r="A424" s="7"/>
       <c r="B424" s="4"/>
       <c r="C424" s="4"/>
-      <c r="D424" s="1"/>
+      <c r="D424" s="4"/>
       <c r="E424" s="4"/>
       <c r="F424" s="4"/>
       <c r="G424" s="5"/>
@@ -4917,7 +4923,7 @@
       <c r="A425" s="7"/>
       <c r="B425" s="4"/>
       <c r="C425" s="4"/>
-      <c r="D425" s="1"/>
+      <c r="D425" s="4"/>
       <c r="E425" s="4"/>
       <c r="F425" s="4"/>
       <c r="G425" s="5"/>
@@ -4927,7 +4933,7 @@
       <c r="A426" s="7"/>
       <c r="B426" s="4"/>
       <c r="C426" s="4"/>
-      <c r="D426" s="1"/>
+      <c r="D426" s="4"/>
       <c r="E426" s="4"/>
       <c r="F426" s="4"/>
       <c r="G426" s="5"/>
@@ -4937,7 +4943,7 @@
       <c r="A427" s="7"/>
       <c r="B427" s="4"/>
       <c r="C427" s="4"/>
-      <c r="D427" s="1"/>
+      <c r="D427" s="4"/>
       <c r="E427" s="4"/>
       <c r="F427" s="4"/>
       <c r="G427" s="5"/>
@@ -4947,7 +4953,7 @@
       <c r="A428" s="7"/>
       <c r="B428" s="4"/>
       <c r="C428" s="4"/>
-      <c r="D428" s="1"/>
+      <c r="D428" s="4"/>
       <c r="E428" s="4"/>
       <c r="F428" s="4"/>
       <c r="G428" s="5"/>
@@ -4957,7 +4963,7 @@
       <c r="A429" s="7"/>
       <c r="B429" s="4"/>
       <c r="C429" s="4"/>
-      <c r="D429" s="1"/>
+      <c r="D429" s="4"/>
       <c r="E429" s="4"/>
       <c r="F429" s="4"/>
       <c r="G429" s="5"/>
@@ -4967,7 +4973,7 @@
       <c r="A430" s="7"/>
       <c r="B430" s="4"/>
       <c r="C430" s="4"/>
-      <c r="D430" s="1"/>
+      <c r="D430" s="4"/>
       <c r="E430" s="4"/>
       <c r="F430" s="4"/>
       <c r="G430" s="5"/>
@@ -4977,7 +4983,7 @@
       <c r="A431" s="7"/>
       <c r="B431" s="4"/>
       <c r="C431" s="4"/>
-      <c r="D431" s="1"/>
+      <c r="D431" s="4"/>
       <c r="E431" s="4"/>
       <c r="F431" s="4"/>
       <c r="G431" s="5"/>
@@ -4987,7 +4993,7 @@
       <c r="A432" s="7"/>
       <c r="B432" s="4"/>
       <c r="C432" s="4"/>
-      <c r="D432" s="1"/>
+      <c r="D432" s="4"/>
       <c r="E432" s="4"/>
       <c r="F432" s="4"/>
       <c r="G432" s="5"/>
@@ -4997,7 +5003,7 @@
       <c r="A433" s="7"/>
       <c r="B433" s="4"/>
       <c r="C433" s="4"/>
-      <c r="D433" s="1"/>
+      <c r="D433" s="4"/>
       <c r="E433" s="4"/>
       <c r="F433" s="4"/>
       <c r="G433" s="5"/>
@@ -5007,7 +5013,7 @@
       <c r="A434" s="7"/>
       <c r="B434" s="4"/>
       <c r="C434" s="4"/>
-      <c r="D434" s="1"/>
+      <c r="D434" s="4"/>
       <c r="E434" s="4"/>
       <c r="F434" s="4"/>
       <c r="G434" s="5"/>
@@ -5017,7 +5023,7 @@
       <c r="A435" s="7"/>
       <c r="B435" s="4"/>
       <c r="C435" s="4"/>
-      <c r="D435" s="1"/>
+      <c r="D435" s="4"/>
       <c r="E435" s="4"/>
       <c r="F435" s="4"/>
       <c r="G435" s="5"/>
@@ -5027,7 +5033,7 @@
       <c r="A436" s="7"/>
       <c r="B436" s="4"/>
       <c r="C436" s="4"/>
-      <c r="D436" s="1"/>
+      <c r="D436" s="4"/>
       <c r="E436" s="4"/>
       <c r="F436" s="4"/>
       <c r="G436" s="5"/>
@@ -5037,7 +5043,7 @@
       <c r="A437" s="7"/>
       <c r="B437" s="4"/>
       <c r="C437" s="4"/>
-      <c r="D437" s="1"/>
+      <c r="D437" s="4"/>
       <c r="E437" s="4"/>
       <c r="F437" s="4"/>
       <c r="G437" s="5"/>
@@ -5047,7 +5053,7 @@
       <c r="A438" s="7"/>
       <c r="B438" s="4"/>
       <c r="C438" s="4"/>
-      <c r="D438" s="1"/>
+      <c r="D438" s="4"/>
       <c r="E438" s="4"/>
       <c r="F438" s="4"/>
       <c r="G438" s="5"/>
@@ -5057,7 +5063,7 @@
       <c r="A439" s="7"/>
       <c r="B439" s="4"/>
       <c r="C439" s="4"/>
-      <c r="D439" s="1"/>
+      <c r="D439" s="4"/>
       <c r="E439" s="4"/>
       <c r="F439" s="4"/>
       <c r="G439" s="5"/>
@@ -5067,7 +5073,7 @@
       <c r="A440" s="7"/>
       <c r="B440" s="4"/>
       <c r="C440" s="4"/>
-      <c r="D440" s="1"/>
+      <c r="D440" s="4"/>
       <c r="E440" s="4"/>
       <c r="F440" s="4"/>
       <c r="G440" s="5"/>
@@ -5077,7 +5083,7 @@
       <c r="A441" s="7"/>
       <c r="B441" s="4"/>
       <c r="C441" s="4"/>
-      <c r="D441" s="1"/>
+      <c r="D441" s="4"/>
       <c r="E441" s="4"/>
       <c r="F441" s="4"/>
       <c r="G441" s="5"/>
@@ -5087,7 +5093,7 @@
       <c r="A442" s="7"/>
       <c r="B442" s="4"/>
       <c r="C442" s="4"/>
-      <c r="D442" s="1"/>
+      <c r="D442" s="4"/>
       <c r="E442" s="4"/>
       <c r="F442" s="4"/>
       <c r="G442" s="5"/>
@@ -5097,7 +5103,7 @@
       <c r="A443" s="7"/>
       <c r="B443" s="4"/>
       <c r="C443" s="4"/>
-      <c r="D443" s="1"/>
+      <c r="D443" s="4"/>
       <c r="E443" s="4"/>
       <c r="F443" s="4"/>
       <c r="G443" s="5"/>
@@ -5107,7 +5113,7 @@
       <c r="A444" s="7"/>
       <c r="B444" s="4"/>
       <c r="C444" s="4"/>
-      <c r="D444" s="1"/>
+      <c r="D444" s="4"/>
       <c r="E444" s="4"/>
       <c r="F444" s="4"/>
       <c r="G444" s="5"/>
@@ -5117,7 +5123,7 @@
       <c r="A445" s="7"/>
       <c r="B445" s="4"/>
       <c r="C445" s="4"/>
-      <c r="D445" s="1"/>
+      <c r="D445" s="4"/>
       <c r="E445" s="4"/>
       <c r="F445" s="4"/>
       <c r="G445" s="5"/>
@@ -9073,290 +9079,290 @@
       <c r="G840" s="5"/>
       <c r="H840" s="5"/>
     </row>
-    <row r="841" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A841" s="7"/>
-      <c r="B841" s="4"/>
-      <c r="C841" s="4"/>
-      <c r="D841" s="4"/>
-      <c r="E841" s="4"/>
-      <c r="F841" s="4"/>
       <c r="G841" s="5"/>
       <c r="H841" s="5"/>
     </row>
-    <row r="842" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A842" s="7"/>
-      <c r="B842" s="4"/>
-      <c r="C842" s="4"/>
-      <c r="D842" s="4"/>
-      <c r="E842" s="4"/>
-      <c r="F842" s="4"/>
       <c r="G842" s="5"/>
       <c r="H842" s="5"/>
     </row>
-    <row r="843" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A843" s="7"/>
-      <c r="B843" s="4"/>
-      <c r="C843" s="4"/>
-      <c r="D843" s="4"/>
-      <c r="E843" s="4"/>
-      <c r="F843" s="4"/>
       <c r="G843" s="5"/>
       <c r="H843" s="5"/>
     </row>
-    <row r="844" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A844" s="7"/>
-      <c r="B844" s="4"/>
-      <c r="C844" s="4"/>
-      <c r="D844" s="4"/>
-      <c r="E844" s="4"/>
-      <c r="F844" s="4"/>
       <c r="G844" s="5"/>
       <c r="H844" s="5"/>
     </row>
-    <row r="845" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A845" s="7"/>
-      <c r="B845" s="4"/>
-      <c r="C845" s="4"/>
-      <c r="D845" s="4"/>
-      <c r="E845" s="4"/>
-      <c r="F845" s="4"/>
       <c r="G845" s="5"/>
       <c r="H845" s="5"/>
     </row>
-    <row r="846" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A846" s="7"/>
-      <c r="B846" s="4"/>
-      <c r="C846" s="4"/>
-      <c r="D846" s="4"/>
-      <c r="E846" s="4"/>
-      <c r="F846" s="4"/>
       <c r="G846" s="5"/>
       <c r="H846" s="5"/>
     </row>
-    <row r="847" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A847" s="7"/>
-      <c r="B847" s="4"/>
-      <c r="C847" s="4"/>
-      <c r="D847" s="4"/>
-      <c r="E847" s="4"/>
-      <c r="F847" s="4"/>
       <c r="G847" s="5"/>
       <c r="H847" s="5"/>
     </row>
-    <row r="848" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A848" s="7"/>
-      <c r="B848" s="4"/>
-      <c r="C848" s="4"/>
-      <c r="D848" s="4"/>
-      <c r="E848" s="4"/>
-      <c r="F848" s="4"/>
       <c r="G848" s="5"/>
       <c r="H848" s="5"/>
     </row>
-    <row r="849" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A849" s="7"/>
-      <c r="B849" s="4"/>
-      <c r="C849" s="4"/>
-      <c r="D849" s="4"/>
-      <c r="E849" s="4"/>
-      <c r="F849" s="4"/>
       <c r="G849" s="5"/>
       <c r="H849" s="5"/>
     </row>
     <row r="850" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A850" s="7"/>
-      <c r="B850" s="4"/>
-      <c r="C850" s="4"/>
-      <c r="D850" s="4"/>
-      <c r="E850" s="4"/>
-      <c r="F850" s="4"/>
-      <c r="G850" s="5"/>
-      <c r="H850" s="5"/>
+      <c r="B850" s="6"/>
+      <c r="C850" s="6"/>
+      <c r="D850" s="6"/>
+      <c r="E850" s="6"/>
+      <c r="F850" s="6"/>
+      <c r="G850" s="8"/>
+      <c r="H850" s="8"/>
     </row>
     <row r="851" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A851" s="7"/>
-      <c r="B851" s="4"/>
-      <c r="C851" s="4"/>
-      <c r="D851" s="4"/>
-      <c r="E851" s="4"/>
-      <c r="F851" s="4"/>
-      <c r="G851" s="5"/>
-      <c r="H851" s="5"/>
+      <c r="B851" s="6"/>
+      <c r="C851" s="6"/>
+      <c r="D851" s="6"/>
+      <c r="E851" s="6"/>
+      <c r="F851" s="6"/>
+      <c r="G851" s="8"/>
+      <c r="H851" s="8"/>
     </row>
     <row r="852" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A852" s="7"/>
-      <c r="B852" s="4"/>
-      <c r="C852" s="4"/>
-      <c r="D852" s="4"/>
-      <c r="E852" s="4"/>
-      <c r="F852" s="4"/>
-      <c r="G852" s="5"/>
-      <c r="H852" s="5"/>
+      <c r="B852" s="6"/>
+      <c r="C852" s="6"/>
+      <c r="D852" s="6"/>
+      <c r="E852" s="6"/>
+      <c r="F852" s="6"/>
+      <c r="G852" s="8"/>
+      <c r="H852" s="8"/>
     </row>
     <row r="853" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A853" s="7"/>
-      <c r="B853" s="4"/>
-      <c r="C853" s="4"/>
-      <c r="D853" s="4"/>
-      <c r="E853" s="4"/>
-      <c r="F853" s="4"/>
-      <c r="G853" s="5"/>
-      <c r="H853" s="5"/>
+      <c r="B853" s="6"/>
+      <c r="C853" s="6"/>
+      <c r="D853" s="6"/>
+      <c r="E853" s="6"/>
+      <c r="F853" s="6"/>
+      <c r="G853" s="8"/>
+      <c r="H853" s="8"/>
     </row>
     <row r="854" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A854" s="7"/>
-      <c r="B854" s="4"/>
-      <c r="C854" s="4"/>
-      <c r="D854" s="4"/>
-      <c r="E854" s="4"/>
-      <c r="F854" s="4"/>
-      <c r="G854" s="5"/>
-      <c r="H854" s="5"/>
+      <c r="B854" s="6"/>
+      <c r="C854" s="6"/>
+      <c r="D854" s="6"/>
+      <c r="E854" s="6"/>
+      <c r="F854" s="6"/>
+      <c r="G854" s="8"/>
+      <c r="H854" s="8"/>
     </row>
     <row r="855" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A855" s="7"/>
-      <c r="B855" s="4"/>
-      <c r="C855" s="4"/>
-      <c r="D855" s="4"/>
-      <c r="E855" s="4"/>
-      <c r="F855" s="4"/>
-      <c r="G855" s="5"/>
-      <c r="H855" s="5"/>
+      <c r="B855" s="6"/>
+      <c r="C855" s="6"/>
+      <c r="D855" s="6"/>
+      <c r="E855" s="6"/>
+      <c r="F855" s="6"/>
+      <c r="G855" s="8"/>
+      <c r="H855" s="8"/>
     </row>
     <row r="856" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A856" s="7"/>
-      <c r="B856" s="4"/>
-      <c r="C856" s="4"/>
-      <c r="D856" s="4"/>
-      <c r="E856" s="4"/>
-      <c r="F856" s="4"/>
-      <c r="G856" s="5"/>
-      <c r="H856" s="5"/>
+      <c r="B856" s="6"/>
+      <c r="C856" s="6"/>
+      <c r="D856" s="6"/>
+      <c r="E856" s="6"/>
+      <c r="F856" s="6"/>
+      <c r="G856" s="8"/>
+      <c r="H856" s="8"/>
     </row>
     <row r="857" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A857" s="7"/>
-      <c r="B857" s="4"/>
-      <c r="C857" s="4"/>
-      <c r="D857" s="4"/>
-      <c r="E857" s="4"/>
-      <c r="F857" s="4"/>
-      <c r="G857" s="5"/>
-      <c r="H857" s="5"/>
+      <c r="B857" s="6"/>
+      <c r="C857" s="6"/>
+      <c r="D857" s="6"/>
+      <c r="E857" s="6"/>
+      <c r="F857" s="6"/>
+      <c r="G857" s="8"/>
+      <c r="H857" s="8"/>
     </row>
     <row r="858" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A858" s="7"/>
-      <c r="B858" s="4"/>
-      <c r="C858" s="4"/>
-      <c r="D858" s="4"/>
-      <c r="E858" s="4"/>
-      <c r="F858" s="4"/>
-      <c r="G858" s="5"/>
-      <c r="H858" s="5"/>
+      <c r="B858" s="6"/>
+      <c r="C858" s="6"/>
+      <c r="D858" s="6"/>
+      <c r="E858" s="6"/>
+      <c r="F858" s="6"/>
+      <c r="G858" s="8"/>
+      <c r="H858" s="8"/>
     </row>
     <row r="859" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A859" s="7"/>
-      <c r="B859" s="4"/>
-      <c r="C859" s="4"/>
-      <c r="D859" s="4"/>
-      <c r="E859" s="4"/>
-      <c r="F859" s="4"/>
-      <c r="G859" s="5"/>
-      <c r="H859" s="5"/>
+      <c r="B859" s="6"/>
+      <c r="C859" s="6"/>
+      <c r="D859" s="6"/>
+      <c r="E859" s="6"/>
+      <c r="F859" s="6"/>
+      <c r="G859" s="8"/>
+      <c r="H859" s="8"/>
     </row>
     <row r="860" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A860" s="7"/>
-      <c r="B860" s="4"/>
-      <c r="C860" s="4"/>
-      <c r="D860" s="4"/>
-      <c r="E860" s="4"/>
-      <c r="F860" s="4"/>
-      <c r="G860" s="5"/>
-      <c r="H860" s="5"/>
+      <c r="B860" s="6"/>
+      <c r="C860" s="6"/>
+      <c r="D860" s="6"/>
+      <c r="E860" s="6"/>
+      <c r="F860" s="6"/>
+      <c r="G860" s="8"/>
+      <c r="H860" s="8"/>
     </row>
     <row r="861" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A861" s="7"/>
-      <c r="B861" s="4"/>
-      <c r="C861" s="4"/>
-      <c r="D861" s="4"/>
-      <c r="E861" s="4"/>
-      <c r="F861" s="4"/>
-      <c r="G861" s="5"/>
-      <c r="H861" s="5"/>
+      <c r="B861" s="6"/>
+      <c r="C861" s="6"/>
+      <c r="D861" s="6"/>
+      <c r="E861" s="6"/>
+      <c r="F861" s="6"/>
+      <c r="G861" s="8"/>
+      <c r="H861" s="8"/>
     </row>
     <row r="862" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A862" s="7"/>
-      <c r="B862" s="4"/>
-      <c r="C862" s="4"/>
-      <c r="D862" s="4"/>
-      <c r="E862" s="4"/>
-      <c r="F862" s="4"/>
-      <c r="G862" s="5"/>
-      <c r="H862" s="5"/>
+      <c r="B862" s="6"/>
+      <c r="C862" s="6"/>
+      <c r="D862" s="6"/>
+      <c r="E862" s="6"/>
+      <c r="F862" s="6"/>
+      <c r="G862" s="8"/>
+      <c r="H862" s="8"/>
     </row>
     <row r="863" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A863" s="7"/>
-      <c r="B863" s="4"/>
-      <c r="C863" s="4"/>
-      <c r="D863" s="4"/>
-      <c r="E863" s="4"/>
-      <c r="F863" s="4"/>
-      <c r="G863" s="5"/>
-      <c r="H863" s="5"/>
+      <c r="B863" s="6"/>
+      <c r="C863" s="6"/>
+      <c r="D863" s="6"/>
+      <c r="E863" s="6"/>
+      <c r="F863" s="6"/>
+      <c r="G863" s="8"/>
+      <c r="H863" s="8"/>
     </row>
     <row r="864" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A864" s="7"/>
-      <c r="B864" s="4"/>
-      <c r="C864" s="4"/>
-      <c r="D864" s="4"/>
-      <c r="E864" s="4"/>
-      <c r="F864" s="4"/>
-      <c r="G864" s="5"/>
-      <c r="H864" s="5"/>
-    </row>
-    <row r="865" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B864" s="6"/>
+      <c r="C864" s="6"/>
+      <c r="D864" s="6"/>
+      <c r="E864" s="6"/>
+      <c r="F864" s="6"/>
+      <c r="G864" s="8"/>
+      <c r="H864" s="8"/>
+    </row>
+    <row r="865" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A865" s="7"/>
-      <c r="G865" s="5"/>
-      <c r="H865" s="5"/>
-    </row>
-    <row r="866" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B865" s="6"/>
+      <c r="C865" s="6"/>
+      <c r="D865" s="6"/>
+      <c r="E865" s="6"/>
+      <c r="F865" s="6"/>
+      <c r="G865" s="8"/>
+      <c r="H865" s="8"/>
+    </row>
+    <row r="866" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A866" s="7"/>
-      <c r="G866" s="5"/>
-      <c r="H866" s="5"/>
-    </row>
-    <row r="867" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B866" s="6"/>
+      <c r="C866" s="6"/>
+      <c r="D866" s="6"/>
+      <c r="E866" s="6"/>
+      <c r="F866" s="6"/>
+      <c r="G866" s="8"/>
+      <c r="H866" s="8"/>
+    </row>
+    <row r="867" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A867" s="7"/>
-      <c r="G867" s="5"/>
-      <c r="H867" s="5"/>
-    </row>
-    <row r="868" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B867" s="6"/>
+      <c r="C867" s="6"/>
+      <c r="D867" s="6"/>
+      <c r="E867" s="6"/>
+      <c r="F867" s="6"/>
+      <c r="G867" s="8"/>
+      <c r="H867" s="8"/>
+    </row>
+    <row r="868" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A868" s="7"/>
-      <c r="G868" s="5"/>
-      <c r="H868" s="5"/>
-    </row>
-    <row r="869" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B868" s="6"/>
+      <c r="C868" s="6"/>
+      <c r="D868" s="6"/>
+      <c r="E868" s="6"/>
+      <c r="F868" s="6"/>
+      <c r="G868" s="8"/>
+      <c r="H868" s="8"/>
+    </row>
+    <row r="869" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A869" s="7"/>
-      <c r="G869" s="5"/>
-      <c r="H869" s="5"/>
-    </row>
-    <row r="870" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B869" s="6"/>
+      <c r="C869" s="6"/>
+      <c r="D869" s="6"/>
+      <c r="E869" s="6"/>
+      <c r="F869" s="6"/>
+      <c r="G869" s="8"/>
+      <c r="H869" s="8"/>
+    </row>
+    <row r="870" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A870" s="7"/>
-      <c r="G870" s="5"/>
-      <c r="H870" s="5"/>
-    </row>
-    <row r="871" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B870" s="6"/>
+      <c r="C870" s="6"/>
+      <c r="D870" s="6"/>
+      <c r="E870" s="6"/>
+      <c r="F870" s="6"/>
+      <c r="G870" s="8"/>
+      <c r="H870" s="8"/>
+    </row>
+    <row r="871" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A871" s="7"/>
-      <c r="G871" s="5"/>
-      <c r="H871" s="5"/>
-    </row>
-    <row r="872" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B871" s="6"/>
+      <c r="C871" s="6"/>
+      <c r="D871" s="6"/>
+      <c r="E871" s="6"/>
+      <c r="F871" s="6"/>
+      <c r="G871" s="8"/>
+      <c r="H871" s="8"/>
+    </row>
+    <row r="872" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A872" s="7"/>
-      <c r="G872" s="5"/>
-      <c r="H872" s="5"/>
-    </row>
-    <row r="873" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B872" s="6"/>
+      <c r="C872" s="6"/>
+      <c r="D872" s="6"/>
+      <c r="E872" s="6"/>
+      <c r="F872" s="6"/>
+      <c r="G872" s="8"/>
+      <c r="H872" s="8"/>
+    </row>
+    <row r="873" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A873" s="7"/>
-      <c r="G873" s="5"/>
-      <c r="H873" s="5"/>
+      <c r="B873" s="6"/>
+      <c r="C873" s="6"/>
+      <c r="D873" s="6"/>
+      <c r="E873" s="6"/>
+      <c r="F873" s="6"/>
+      <c r="G873" s="8"/>
+      <c r="H873" s="8"/>
     </row>
     <row r="874" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A874" s="7"/>
@@ -14508,7 +14514,7 @@
       <c r="G1388" s="8"/>
       <c r="H1388" s="8"/>
     </row>
-    <row r="1389" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1389" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1389" s="7"/>
       <c r="B1389" s="6"/>
       <c r="C1389" s="6"/>
@@ -14518,7 +14524,7 @@
       <c r="G1389" s="8"/>
       <c r="H1389" s="8"/>
     </row>
-    <row r="1390" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1390" s="7"/>
       <c r="B1390" s="6"/>
       <c r="C1390" s="6"/>
@@ -14528,7 +14534,7 @@
       <c r="G1390" s="8"/>
       <c r="H1390" s="8"/>
     </row>
-    <row r="1391" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1391" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1391" s="7"/>
       <c r="B1391" s="6"/>
       <c r="C1391" s="6"/>
@@ -14538,7 +14544,7 @@
       <c r="G1391" s="8"/>
       <c r="H1391" s="8"/>
     </row>
-    <row r="1392" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1392" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1392" s="7"/>
       <c r="B1392" s="6"/>
       <c r="C1392" s="6"/>
@@ -14548,7 +14554,7 @@
       <c r="G1392" s="8"/>
       <c r="H1392" s="8"/>
     </row>
-    <row r="1393" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1393" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1393" s="7"/>
       <c r="B1393" s="6"/>
       <c r="C1393" s="6"/>
@@ -14558,7 +14564,7 @@
       <c r="G1393" s="8"/>
       <c r="H1393" s="8"/>
     </row>
-    <row r="1394" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1394" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1394" s="7"/>
       <c r="B1394" s="6"/>
       <c r="C1394" s="6"/>
@@ -14568,7 +14574,7 @@
       <c r="G1394" s="8"/>
       <c r="H1394" s="8"/>
     </row>
-    <row r="1395" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1395" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1395" s="7"/>
       <c r="B1395" s="6"/>
       <c r="C1395" s="6"/>
@@ -14578,7 +14584,7 @@
       <c r="G1395" s="8"/>
       <c r="H1395" s="8"/>
     </row>
-    <row r="1396" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1396" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1396" s="7"/>
       <c r="B1396" s="6"/>
       <c r="C1396" s="6"/>
@@ -14588,7 +14594,7 @@
       <c r="G1396" s="8"/>
       <c r="H1396" s="8"/>
     </row>
-    <row r="1397" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1397" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1397" s="7"/>
       <c r="B1397" s="6"/>
       <c r="C1397" s="6"/>
@@ -14748,7 +14754,7 @@
       <c r="G1412" s="8"/>
       <c r="H1412" s="8"/>
     </row>
-    <row r="1413" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1413" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1413" s="7"/>
       <c r="B1413" s="6"/>
       <c r="C1413" s="6"/>
@@ -14758,7 +14764,7 @@
       <c r="G1413" s="8"/>
       <c r="H1413" s="8"/>
     </row>
-    <row r="1414" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1414" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1414" s="7"/>
       <c r="B1414" s="6"/>
       <c r="C1414" s="6"/>
@@ -14768,7 +14774,7 @@
       <c r="G1414" s="8"/>
       <c r="H1414" s="8"/>
     </row>
-    <row r="1415" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1415" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1415" s="7"/>
       <c r="B1415" s="6"/>
       <c r="C1415" s="6"/>
@@ -14778,7 +14784,7 @@
       <c r="G1415" s="8"/>
       <c r="H1415" s="8"/>
     </row>
-    <row r="1416" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1416" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1416" s="7"/>
       <c r="B1416" s="6"/>
       <c r="C1416" s="6"/>
@@ -14788,7 +14794,7 @@
       <c r="G1416" s="8"/>
       <c r="H1416" s="8"/>
     </row>
-    <row r="1417" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1417" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1417" s="7"/>
       <c r="B1417" s="6"/>
       <c r="C1417" s="6"/>
@@ -14798,7 +14804,7 @@
       <c r="G1417" s="8"/>
       <c r="H1417" s="8"/>
     </row>
-    <row r="1418" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1418" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1418" s="7"/>
       <c r="B1418" s="6"/>
       <c r="C1418" s="6"/>
@@ -14808,7 +14814,7 @@
       <c r="G1418" s="8"/>
       <c r="H1418" s="8"/>
     </row>
-    <row r="1419" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1419" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1419" s="7"/>
       <c r="B1419" s="6"/>
       <c r="C1419" s="6"/>
@@ -14818,7 +14824,7 @@
       <c r="G1419" s="8"/>
       <c r="H1419" s="8"/>
     </row>
-    <row r="1420" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1420" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1420" s="7"/>
       <c r="B1420" s="6"/>
       <c r="C1420" s="6"/>
@@ -14828,7 +14834,7 @@
       <c r="G1420" s="8"/>
       <c r="H1420" s="8"/>
     </row>
-    <row r="1421" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1421" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1421" s="7"/>
       <c r="B1421" s="6"/>
       <c r="C1421" s="6"/>
@@ -15139,244 +15145,244 @@
       <c r="H1451" s="8"/>
     </row>
     <row r="1452" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1452" s="7"/>
-      <c r="B1452" s="6"/>
-      <c r="C1452" s="6"/>
-      <c r="D1452" s="6"/>
-      <c r="E1452" s="6"/>
-      <c r="F1452" s="6"/>
-      <c r="G1452" s="8"/>
-      <c r="H1452" s="8"/>
+      <c r="A1452" s="3"/>
+      <c r="B1452" s="4"/>
+      <c r="C1452" s="4"/>
+      <c r="D1452" s="4"/>
+      <c r="E1452" s="4"/>
+      <c r="F1452" s="4"/>
+      <c r="G1452" s="5"/>
+      <c r="H1452" s="5"/>
     </row>
     <row r="1453" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1453" s="7"/>
-      <c r="B1453" s="6"/>
-      <c r="C1453" s="6"/>
-      <c r="D1453" s="6"/>
-      <c r="E1453" s="6"/>
-      <c r="F1453" s="6"/>
-      <c r="G1453" s="8"/>
-      <c r="H1453" s="8"/>
+      <c r="A1453" s="3"/>
+      <c r="B1453" s="4"/>
+      <c r="C1453" s="4"/>
+      <c r="D1453" s="4"/>
+      <c r="E1453" s="4"/>
+      <c r="F1453" s="4"/>
+      <c r="G1453" s="5"/>
+      <c r="H1453" s="5"/>
     </row>
     <row r="1454" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1454" s="7"/>
-      <c r="B1454" s="6"/>
-      <c r="C1454" s="6"/>
-      <c r="D1454" s="6"/>
-      <c r="E1454" s="6"/>
-      <c r="F1454" s="6"/>
-      <c r="G1454" s="8"/>
-      <c r="H1454" s="8"/>
+      <c r="A1454" s="3"/>
+      <c r="B1454" s="4"/>
+      <c r="C1454" s="4"/>
+      <c r="D1454" s="4"/>
+      <c r="E1454" s="4"/>
+      <c r="F1454" s="4"/>
+      <c r="G1454" s="5"/>
+      <c r="H1454" s="5"/>
     </row>
     <row r="1455" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1455" s="7"/>
-      <c r="B1455" s="6"/>
-      <c r="C1455" s="6"/>
-      <c r="D1455" s="6"/>
-      <c r="E1455" s="6"/>
-      <c r="F1455" s="6"/>
-      <c r="G1455" s="8"/>
-      <c r="H1455" s="8"/>
+      <c r="A1455" s="3"/>
+      <c r="B1455" s="4"/>
+      <c r="C1455" s="4"/>
+      <c r="D1455" s="4"/>
+      <c r="E1455" s="4"/>
+      <c r="F1455" s="4"/>
+      <c r="G1455" s="5"/>
+      <c r="H1455" s="5"/>
     </row>
     <row r="1456" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1456" s="7"/>
-      <c r="B1456" s="6"/>
-      <c r="C1456" s="6"/>
-      <c r="D1456" s="6"/>
-      <c r="E1456" s="6"/>
-      <c r="F1456" s="6"/>
-      <c r="G1456" s="8"/>
-      <c r="H1456" s="8"/>
+      <c r="A1456" s="3"/>
+      <c r="B1456" s="4"/>
+      <c r="C1456" s="4"/>
+      <c r="D1456" s="4"/>
+      <c r="E1456" s="4"/>
+      <c r="F1456" s="4"/>
+      <c r="G1456" s="5"/>
+      <c r="H1456" s="5"/>
     </row>
     <row r="1457" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1457" s="7"/>
-      <c r="B1457" s="6"/>
-      <c r="C1457" s="6"/>
-      <c r="D1457" s="6"/>
-      <c r="E1457" s="6"/>
-      <c r="F1457" s="6"/>
-      <c r="G1457" s="8"/>
-      <c r="H1457" s="8"/>
+      <c r="A1457" s="3"/>
+      <c r="B1457" s="4"/>
+      <c r="C1457" s="4"/>
+      <c r="D1457" s="4"/>
+      <c r="E1457" s="4"/>
+      <c r="F1457" s="4"/>
+      <c r="G1457" s="5"/>
+      <c r="H1457" s="5"/>
     </row>
     <row r="1458" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1458" s="7"/>
-      <c r="B1458" s="6"/>
-      <c r="C1458" s="6"/>
-      <c r="D1458" s="6"/>
-      <c r="E1458" s="6"/>
-      <c r="F1458" s="6"/>
-      <c r="G1458" s="8"/>
-      <c r="H1458" s="8"/>
+      <c r="A1458" s="3"/>
+      <c r="B1458" s="4"/>
+      <c r="C1458" s="4"/>
+      <c r="D1458" s="4"/>
+      <c r="E1458" s="4"/>
+      <c r="F1458" s="4"/>
+      <c r="G1458" s="5"/>
+      <c r="H1458" s="5"/>
     </row>
     <row r="1459" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1459" s="7"/>
-      <c r="B1459" s="6"/>
-      <c r="C1459" s="6"/>
-      <c r="D1459" s="6"/>
-      <c r="E1459" s="6"/>
-      <c r="F1459" s="6"/>
-      <c r="G1459" s="8"/>
-      <c r="H1459" s="8"/>
+      <c r="A1459" s="3"/>
+      <c r="B1459" s="4"/>
+      <c r="C1459" s="4"/>
+      <c r="D1459" s="4"/>
+      <c r="E1459" s="4"/>
+      <c r="F1459" s="4"/>
+      <c r="G1459" s="5"/>
+      <c r="H1459" s="5"/>
     </row>
     <row r="1460" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1460" s="7"/>
-      <c r="B1460" s="6"/>
-      <c r="C1460" s="6"/>
-      <c r="D1460" s="6"/>
-      <c r="E1460" s="6"/>
-      <c r="F1460" s="6"/>
-      <c r="G1460" s="8"/>
-      <c r="H1460" s="8"/>
+      <c r="A1460" s="3"/>
+      <c r="B1460" s="4"/>
+      <c r="C1460" s="4"/>
+      <c r="D1460" s="4"/>
+      <c r="E1460" s="4"/>
+      <c r="F1460" s="4"/>
+      <c r="G1460" s="5"/>
+      <c r="H1460" s="5"/>
     </row>
     <row r="1461" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1461" s="7"/>
-      <c r="B1461" s="6"/>
-      <c r="C1461" s="6"/>
-      <c r="D1461" s="6"/>
-      <c r="E1461" s="6"/>
-      <c r="F1461" s="6"/>
-      <c r="G1461" s="8"/>
-      <c r="H1461" s="8"/>
+      <c r="A1461" s="3"/>
+      <c r="B1461" s="4"/>
+      <c r="C1461" s="4"/>
+      <c r="D1461" s="4"/>
+      <c r="E1461" s="4"/>
+      <c r="F1461" s="4"/>
+      <c r="G1461" s="5"/>
+      <c r="H1461" s="5"/>
     </row>
     <row r="1462" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1462" s="7"/>
-      <c r="B1462" s="6"/>
-      <c r="C1462" s="6"/>
-      <c r="D1462" s="6"/>
-      <c r="E1462" s="6"/>
-      <c r="F1462" s="6"/>
-      <c r="G1462" s="8"/>
-      <c r="H1462" s="8"/>
+      <c r="A1462" s="3"/>
+      <c r="B1462" s="4"/>
+      <c r="C1462" s="4"/>
+      <c r="D1462" s="4"/>
+      <c r="E1462" s="4"/>
+      <c r="F1462" s="4"/>
+      <c r="G1462" s="5"/>
+      <c r="H1462" s="5"/>
     </row>
     <row r="1463" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1463" s="7"/>
-      <c r="B1463" s="6"/>
-      <c r="C1463" s="6"/>
-      <c r="D1463" s="6"/>
-      <c r="E1463" s="6"/>
-      <c r="F1463" s="6"/>
-      <c r="G1463" s="8"/>
-      <c r="H1463" s="8"/>
+      <c r="A1463" s="3"/>
+      <c r="B1463" s="4"/>
+      <c r="C1463" s="4"/>
+      <c r="D1463" s="4"/>
+      <c r="E1463" s="4"/>
+      <c r="F1463" s="4"/>
+      <c r="G1463" s="5"/>
+      <c r="H1463" s="5"/>
     </row>
     <row r="1464" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1464" s="7"/>
-      <c r="B1464" s="6"/>
-      <c r="C1464" s="6"/>
-      <c r="D1464" s="6"/>
-      <c r="E1464" s="6"/>
-      <c r="F1464" s="6"/>
-      <c r="G1464" s="8"/>
-      <c r="H1464" s="8"/>
+      <c r="A1464" s="3"/>
+      <c r="B1464" s="4"/>
+      <c r="C1464" s="4"/>
+      <c r="D1464" s="4"/>
+      <c r="E1464" s="4"/>
+      <c r="F1464" s="4"/>
+      <c r="G1464" s="5"/>
+      <c r="H1464" s="5"/>
     </row>
     <row r="1465" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1465" s="7"/>
-      <c r="B1465" s="6"/>
-      <c r="C1465" s="6"/>
-      <c r="D1465" s="6"/>
-      <c r="E1465" s="6"/>
-      <c r="F1465" s="6"/>
-      <c r="G1465" s="8"/>
-      <c r="H1465" s="8"/>
+      <c r="A1465" s="3"/>
+      <c r="B1465" s="4"/>
+      <c r="C1465" s="4"/>
+      <c r="D1465" s="4"/>
+      <c r="E1465" s="4"/>
+      <c r="F1465" s="4"/>
+      <c r="G1465" s="5"/>
+      <c r="H1465" s="5"/>
     </row>
     <row r="1466" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1466" s="7"/>
-      <c r="B1466" s="6"/>
-      <c r="C1466" s="6"/>
-      <c r="D1466" s="6"/>
-      <c r="E1466" s="6"/>
-      <c r="F1466" s="6"/>
-      <c r="G1466" s="8"/>
-      <c r="H1466" s="8"/>
+      <c r="A1466" s="3"/>
+      <c r="B1466" s="4"/>
+      <c r="C1466" s="4"/>
+      <c r="D1466" s="4"/>
+      <c r="E1466" s="4"/>
+      <c r="F1466" s="4"/>
+      <c r="G1466" s="5"/>
+      <c r="H1466" s="5"/>
     </row>
     <row r="1467" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1467" s="7"/>
-      <c r="B1467" s="6"/>
-      <c r="C1467" s="6"/>
-      <c r="D1467" s="6"/>
-      <c r="E1467" s="6"/>
-      <c r="F1467" s="6"/>
-      <c r="G1467" s="8"/>
-      <c r="H1467" s="8"/>
+      <c r="A1467" s="3"/>
+      <c r="B1467" s="4"/>
+      <c r="C1467" s="4"/>
+      <c r="D1467" s="4"/>
+      <c r="E1467" s="4"/>
+      <c r="F1467" s="4"/>
+      <c r="G1467" s="5"/>
+      <c r="H1467" s="5"/>
     </row>
     <row r="1468" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1468" s="7"/>
-      <c r="B1468" s="6"/>
-      <c r="C1468" s="6"/>
-      <c r="D1468" s="6"/>
-      <c r="E1468" s="6"/>
-      <c r="F1468" s="6"/>
-      <c r="G1468" s="8"/>
-      <c r="H1468" s="8"/>
+      <c r="A1468" s="3"/>
+      <c r="B1468" s="4"/>
+      <c r="C1468" s="4"/>
+      <c r="D1468" s="4"/>
+      <c r="E1468" s="4"/>
+      <c r="F1468" s="4"/>
+      <c r="G1468" s="5"/>
+      <c r="H1468" s="5"/>
     </row>
     <row r="1469" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1469" s="7"/>
-      <c r="B1469" s="6"/>
-      <c r="C1469" s="6"/>
-      <c r="D1469" s="6"/>
-      <c r="E1469" s="6"/>
-      <c r="F1469" s="6"/>
-      <c r="G1469" s="8"/>
-      <c r="H1469" s="8"/>
+      <c r="A1469" s="3"/>
+      <c r="B1469" s="4"/>
+      <c r="C1469" s="4"/>
+      <c r="D1469" s="4"/>
+      <c r="E1469" s="4"/>
+      <c r="F1469" s="4"/>
+      <c r="G1469" s="5"/>
+      <c r="H1469" s="5"/>
     </row>
     <row r="1470" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1470" s="7"/>
-      <c r="B1470" s="6"/>
-      <c r="C1470" s="6"/>
-      <c r="D1470" s="6"/>
-      <c r="E1470" s="6"/>
-      <c r="F1470" s="6"/>
-      <c r="G1470" s="8"/>
-      <c r="H1470" s="8"/>
+      <c r="A1470" s="3"/>
+      <c r="B1470" s="4"/>
+      <c r="C1470" s="4"/>
+      <c r="D1470" s="4"/>
+      <c r="E1470" s="4"/>
+      <c r="F1470" s="4"/>
+      <c r="G1470" s="5"/>
+      <c r="H1470" s="5"/>
     </row>
     <row r="1471" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1471" s="7"/>
-      <c r="B1471" s="6"/>
-      <c r="C1471" s="6"/>
-      <c r="D1471" s="6"/>
-      <c r="E1471" s="6"/>
-      <c r="F1471" s="6"/>
-      <c r="G1471" s="8"/>
-      <c r="H1471" s="8"/>
+      <c r="A1471" s="3"/>
+      <c r="B1471" s="4"/>
+      <c r="C1471" s="4"/>
+      <c r="D1471" s="4"/>
+      <c r="E1471" s="4"/>
+      <c r="F1471" s="4"/>
+      <c r="G1471" s="5"/>
+      <c r="H1471" s="5"/>
     </row>
     <row r="1472" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1472" s="7"/>
-      <c r="B1472" s="6"/>
-      <c r="C1472" s="6"/>
-      <c r="D1472" s="6"/>
-      <c r="E1472" s="6"/>
-      <c r="F1472" s="6"/>
-      <c r="G1472" s="8"/>
-      <c r="H1472" s="8"/>
+      <c r="A1472" s="3"/>
+      <c r="B1472" s="4"/>
+      <c r="C1472" s="4"/>
+      <c r="D1472" s="4"/>
+      <c r="E1472" s="4"/>
+      <c r="F1472" s="4"/>
+      <c r="G1472" s="5"/>
+      <c r="H1472" s="5"/>
     </row>
     <row r="1473" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1473" s="7"/>
-      <c r="B1473" s="6"/>
-      <c r="C1473" s="6"/>
-      <c r="D1473" s="6"/>
-      <c r="E1473" s="6"/>
-      <c r="F1473" s="6"/>
-      <c r="G1473" s="8"/>
-      <c r="H1473" s="8"/>
+      <c r="A1473" s="3"/>
+      <c r="B1473" s="4"/>
+      <c r="C1473" s="4"/>
+      <c r="D1473" s="4"/>
+      <c r="E1473" s="4"/>
+      <c r="F1473" s="4"/>
+      <c r="G1473" s="5"/>
+      <c r="H1473" s="5"/>
     </row>
     <row r="1474" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1474" s="7"/>
-      <c r="B1474" s="6"/>
-      <c r="C1474" s="6"/>
-      <c r="D1474" s="6"/>
-      <c r="E1474" s="6"/>
-      <c r="F1474" s="6"/>
-      <c r="G1474" s="8"/>
-      <c r="H1474" s="8"/>
+      <c r="A1474" s="3"/>
+      <c r="B1474" s="4"/>
+      <c r="C1474" s="4"/>
+      <c r="D1474" s="4"/>
+      <c r="E1474" s="4"/>
+      <c r="F1474" s="4"/>
+      <c r="G1474" s="5"/>
+      <c r="H1474" s="5"/>
     </row>
     <row r="1475" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1475" s="7"/>
-      <c r="B1475" s="6"/>
-      <c r="C1475" s="6"/>
-      <c r="D1475" s="6"/>
-      <c r="E1475" s="6"/>
-      <c r="F1475" s="6"/>
-      <c r="G1475" s="8"/>
-      <c r="H1475" s="8"/>
+      <c r="A1475" s="3"/>
+      <c r="B1475" s="4"/>
+      <c r="C1475" s="4"/>
+      <c r="D1475" s="4"/>
+      <c r="E1475" s="4"/>
+      <c r="F1475" s="4"/>
+      <c r="G1475" s="5"/>
+      <c r="H1475" s="5"/>
     </row>
     <row r="1476" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1476" s="3"/>
@@ -17153,7 +17159,7 @@
       <c r="B1653" s="4"/>
       <c r="C1653" s="4"/>
       <c r="D1653" s="4"/>
-      <c r="E1653" s="4"/>
+      <c r="E1653" s="6"/>
       <c r="F1653" s="4"/>
       <c r="G1653" s="5"/>
       <c r="H1653" s="5"/>
@@ -17208,243 +17214,123 @@
       <c r="G1658" s="5"/>
       <c r="H1658" s="5"/>
     </row>
-    <row r="1659" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1659" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1659" s="3"/>
-      <c r="B1659" s="4"/>
-      <c r="C1659" s="4"/>
-      <c r="D1659" s="4"/>
-      <c r="E1659" s="4"/>
-      <c r="F1659" s="4"/>
       <c r="G1659" s="5"/>
       <c r="H1659" s="5"/>
     </row>
-    <row r="1660" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1660" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1660" s="3"/>
-      <c r="B1660" s="4"/>
-      <c r="C1660" s="4"/>
-      <c r="D1660" s="4"/>
-      <c r="E1660" s="4"/>
-      <c r="F1660" s="4"/>
       <c r="G1660" s="5"/>
       <c r="H1660" s="5"/>
     </row>
-    <row r="1661" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1661" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1661" s="3"/>
-      <c r="B1661" s="4"/>
-      <c r="C1661" s="4"/>
-      <c r="D1661" s="4"/>
-      <c r="E1661" s="4"/>
-      <c r="F1661" s="4"/>
       <c r="G1661" s="5"/>
       <c r="H1661" s="5"/>
     </row>
-    <row r="1662" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1662" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1662" s="3"/>
-      <c r="B1662" s="4"/>
-      <c r="C1662" s="4"/>
-      <c r="D1662" s="4"/>
-      <c r="E1662" s="4"/>
-      <c r="F1662" s="4"/>
       <c r="G1662" s="5"/>
       <c r="H1662" s="5"/>
     </row>
-    <row r="1663" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1663" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1663" s="3"/>
-      <c r="B1663" s="4"/>
-      <c r="C1663" s="4"/>
-      <c r="D1663" s="4"/>
-      <c r="E1663" s="4"/>
-      <c r="F1663" s="4"/>
       <c r="G1663" s="5"/>
       <c r="H1663" s="5"/>
     </row>
-    <row r="1664" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1664" s="3"/>
-      <c r="B1664" s="4"/>
-      <c r="C1664" s="4"/>
-      <c r="D1664" s="4"/>
-      <c r="E1664" s="4"/>
-      <c r="F1664" s="4"/>
       <c r="G1664" s="5"/>
       <c r="H1664" s="5"/>
     </row>
-    <row r="1665" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1665" s="3"/>
-      <c r="B1665" s="4"/>
-      <c r="C1665" s="4"/>
-      <c r="D1665" s="4"/>
-      <c r="E1665" s="4"/>
-      <c r="F1665" s="4"/>
       <c r="G1665" s="5"/>
       <c r="H1665" s="5"/>
     </row>
-    <row r="1666" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1666" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1666" s="3"/>
-      <c r="B1666" s="4"/>
-      <c r="C1666" s="4"/>
-      <c r="D1666" s="4"/>
-      <c r="E1666" s="4"/>
-      <c r="F1666" s="4"/>
       <c r="G1666" s="5"/>
       <c r="H1666" s="5"/>
     </row>
-    <row r="1667" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1667" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1667" s="3"/>
-      <c r="B1667" s="4"/>
-      <c r="C1667" s="4"/>
-      <c r="D1667" s="4"/>
-      <c r="E1667" s="4"/>
-      <c r="F1667" s="4"/>
       <c r="G1667" s="5"/>
       <c r="H1667" s="5"/>
     </row>
-    <row r="1668" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1668" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1668" s="3"/>
-      <c r="B1668" s="4"/>
-      <c r="C1668" s="4"/>
-      <c r="D1668" s="4"/>
-      <c r="E1668" s="4"/>
-      <c r="F1668" s="4"/>
       <c r="G1668" s="5"/>
       <c r="H1668" s="5"/>
     </row>
-    <row r="1669" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1669" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1669" s="3"/>
-      <c r="B1669" s="4"/>
-      <c r="C1669" s="4"/>
-      <c r="D1669" s="4"/>
-      <c r="E1669" s="4"/>
-      <c r="F1669" s="4"/>
       <c r="G1669" s="5"/>
       <c r="H1669" s="5"/>
     </row>
-    <row r="1670" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1670" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1670" s="3"/>
-      <c r="B1670" s="4"/>
-      <c r="C1670" s="4"/>
-      <c r="D1670" s="4"/>
-      <c r="E1670" s="4"/>
-      <c r="F1670" s="4"/>
       <c r="G1670" s="5"/>
       <c r="H1670" s="5"/>
     </row>
-    <row r="1671" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1671" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1671" s="3"/>
-      <c r="B1671" s="4"/>
-      <c r="C1671" s="4"/>
-      <c r="D1671" s="4"/>
-      <c r="E1671" s="4"/>
-      <c r="F1671" s="4"/>
       <c r="G1671" s="5"/>
       <c r="H1671" s="5"/>
     </row>
-    <row r="1672" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1672" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1672" s="3"/>
-      <c r="B1672" s="4"/>
-      <c r="C1672" s="4"/>
-      <c r="D1672" s="4"/>
-      <c r="E1672" s="4"/>
-      <c r="F1672" s="4"/>
       <c r="G1672" s="5"/>
       <c r="H1672" s="5"/>
     </row>
-    <row r="1673" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1673" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1673" s="3"/>
-      <c r="B1673" s="4"/>
-      <c r="C1673" s="4"/>
-      <c r="D1673" s="4"/>
-      <c r="E1673" s="4"/>
-      <c r="F1673" s="4"/>
       <c r="G1673" s="5"/>
       <c r="H1673" s="5"/>
     </row>
-    <row r="1674" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1674" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1674" s="3"/>
-      <c r="B1674" s="4"/>
-      <c r="C1674" s="4"/>
-      <c r="D1674" s="4"/>
-      <c r="E1674" s="4"/>
-      <c r="F1674" s="4"/>
       <c r="G1674" s="5"/>
       <c r="H1674" s="5"/>
     </row>
-    <row r="1675" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1675" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1675" s="3"/>
-      <c r="B1675" s="4"/>
-      <c r="C1675" s="4"/>
-      <c r="D1675" s="4"/>
-      <c r="E1675" s="4"/>
-      <c r="F1675" s="4"/>
       <c r="G1675" s="5"/>
       <c r="H1675" s="5"/>
     </row>
-    <row r="1676" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1676" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1676" s="3"/>
-      <c r="B1676" s="4"/>
-      <c r="C1676" s="4"/>
-      <c r="D1676" s="4"/>
-      <c r="E1676" s="4"/>
-      <c r="F1676" s="4"/>
       <c r="G1676" s="5"/>
       <c r="H1676" s="5"/>
     </row>
-    <row r="1677" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1677" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1677" s="3"/>
-      <c r="B1677" s="4"/>
-      <c r="C1677" s="4"/>
-      <c r="D1677" s="4"/>
-      <c r="E1677" s="6"/>
-      <c r="F1677" s="4"/>
       <c r="G1677" s="5"/>
       <c r="H1677" s="5"/>
     </row>
-    <row r="1678" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1678" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1678" s="3"/>
-      <c r="B1678" s="4"/>
-      <c r="C1678" s="4"/>
-      <c r="D1678" s="4"/>
-      <c r="E1678" s="4"/>
-      <c r="F1678" s="4"/>
       <c r="G1678" s="5"/>
       <c r="H1678" s="5"/>
     </row>
-    <row r="1679" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1679" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1679" s="3"/>
-      <c r="B1679" s="4"/>
-      <c r="C1679" s="4"/>
-      <c r="D1679" s="4"/>
-      <c r="E1679" s="4"/>
-      <c r="F1679" s="4"/>
       <c r="G1679" s="5"/>
       <c r="H1679" s="5"/>
     </row>
-    <row r="1680" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1680" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1680" s="3"/>
-      <c r="B1680" s="4"/>
-      <c r="C1680" s="4"/>
-      <c r="D1680" s="4"/>
-      <c r="E1680" s="4"/>
-      <c r="F1680" s="4"/>
       <c r="G1680" s="5"/>
       <c r="H1680" s="5"/>
     </row>
-    <row r="1681" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1681" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1681" s="3"/>
-      <c r="B1681" s="4"/>
-      <c r="C1681" s="4"/>
-      <c r="D1681" s="4"/>
-      <c r="E1681" s="4"/>
-      <c r="F1681" s="4"/>
       <c r="G1681" s="5"/>
       <c r="H1681" s="5"/>
     </row>
-    <row r="1682" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1682" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1682" s="3"/>
-      <c r="B1682" s="4"/>
-      <c r="C1682" s="4"/>
-      <c r="D1682" s="4"/>
-      <c r="E1682" s="4"/>
-      <c r="F1682" s="4"/>
       <c r="G1682" s="5"/>
       <c r="H1682" s="5"/>
     </row>
@@ -19698,129 +19584,9 @@
       <c r="G2132" s="5"/>
       <c r="H2132" s="5"/>
     </row>
-    <row r="2133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2133" s="3"/>
-      <c r="G2133" s="5"/>
-      <c r="H2133" s="5"/>
-    </row>
-    <row r="2134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2134" s="3"/>
-      <c r="G2134" s="5"/>
-      <c r="H2134" s="5"/>
-    </row>
-    <row r="2135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2135" s="3"/>
-      <c r="G2135" s="5"/>
-      <c r="H2135" s="5"/>
-    </row>
-    <row r="2136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2136" s="3"/>
-      <c r="G2136" s="5"/>
-      <c r="H2136" s="5"/>
-    </row>
-    <row r="2137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2137" s="3"/>
-      <c r="G2137" s="5"/>
-      <c r="H2137" s="5"/>
-    </row>
-    <row r="2138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2138" s="3"/>
-      <c r="G2138" s="5"/>
-      <c r="H2138" s="5"/>
-    </row>
-    <row r="2139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2139" s="3"/>
-      <c r="G2139" s="5"/>
-      <c r="H2139" s="5"/>
-    </row>
-    <row r="2140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2140" s="3"/>
-      <c r="G2140" s="5"/>
-      <c r="H2140" s="5"/>
-    </row>
-    <row r="2141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2141" s="3"/>
-      <c r="G2141" s="5"/>
-      <c r="H2141" s="5"/>
-    </row>
-    <row r="2142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2142" s="3"/>
-      <c r="G2142" s="5"/>
-      <c r="H2142" s="5"/>
-    </row>
-    <row r="2143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2143" s="3"/>
-      <c r="G2143" s="5"/>
-      <c r="H2143" s="5"/>
-    </row>
-    <row r="2144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2144" s="3"/>
-      <c r="G2144" s="5"/>
-      <c r="H2144" s="5"/>
-    </row>
-    <row r="2145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2145" s="3"/>
-      <c r="G2145" s="5"/>
-      <c r="H2145" s="5"/>
-    </row>
-    <row r="2146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2146" s="3"/>
-      <c r="G2146" s="5"/>
-      <c r="H2146" s="5"/>
-    </row>
-    <row r="2147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2147" s="3"/>
-      <c r="G2147" s="5"/>
-      <c r="H2147" s="5"/>
-    </row>
-    <row r="2148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2148" s="3"/>
-      <c r="G2148" s="5"/>
-      <c r="H2148" s="5"/>
-    </row>
-    <row r="2149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2149" s="3"/>
-      <c r="G2149" s="5"/>
-      <c r="H2149" s="5"/>
-    </row>
-    <row r="2150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2150" s="3"/>
-      <c r="G2150" s="5"/>
-      <c r="H2150" s="5"/>
-    </row>
-    <row r="2151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2151" s="3"/>
-      <c r="G2151" s="5"/>
-      <c r="H2151" s="5"/>
-    </row>
-    <row r="2152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2152" s="3"/>
-      <c r="G2152" s="5"/>
-      <c r="H2152" s="5"/>
-    </row>
-    <row r="2153" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2153" s="3"/>
-      <c r="G2153" s="5"/>
-      <c r="H2153" s="5"/>
-    </row>
-    <row r="2154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2154" s="3"/>
-      <c r="G2154" s="5"/>
-      <c r="H2154" s="5"/>
-    </row>
-    <row r="2155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2155" s="3"/>
-      <c r="G2155" s="5"/>
-      <c r="H2155" s="5"/>
-    </row>
-    <row r="2156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2156" s="3"/>
-      <c r="G2156" s="5"/>
-      <c r="H2156" s="5"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H338">
-    <sortCondition descending="1" ref="A1:A338"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H314">
+    <sortCondition descending="1" ref="A1:A314"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>